<commit_message>
More code modifications plus level 1 and 2 files for selected countries
</commit_message>
<xml_diff>
--- a/data-raw/regionInformation/wg2ch5Locations.xlsx
+++ b/data-raw/regionInformation/wg2ch5Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/ISIMIPData/data-raw/regionInformation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D9DDB6-F981-FB48-9647-CCA89893D166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E71F57B-A03C-1946-9517-7D00CDE52AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5140" yWindow="21560" windowWidth="34940" windowHeight="15440" xr2:uid="{02F4FA97-6E90-D04F-8B97-AC9F3BC53EA0}"/>
   </bookViews>
@@ -635,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B950FA-0A16-3042-B472-F300234D4FE0}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,19 +709,19 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="4">
-        <f t="shared" ref="G2:G15" si="0">ROUND(D2-B$18, 0)</f>
+        <f>ROUND(D2-B$17, 0)</f>
         <v>-35</v>
       </c>
       <c r="H2" s="4">
-        <f t="shared" ref="H2:H15" si="1">ROUND(E2-$B$18, 0)</f>
+        <f>ROUND(E2-$B$17, 0)</f>
         <v>-73</v>
       </c>
       <c r="I2" s="4">
-        <f t="shared" ref="I2:I15" si="2">ROUND(D2+B$18, 0)</f>
+        <f>ROUND(D2+B$17, 0)</f>
         <v>-31</v>
       </c>
       <c r="J2" s="4">
-        <f t="shared" ref="J2:J15" si="3">ROUND(E2+B$18, 0)</f>
+        <f>ROUND(E2+B$17, 0)</f>
         <v>-69</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -746,19 +746,19 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(D3-B$17, 0)</f>
         <v>40</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" si="1"/>
+        <f>ROUND(E3-$B$17, 0)</f>
         <v>-78</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" si="2"/>
+        <f>ROUND(D3+B$17, 0)</f>
         <v>44</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" si="3"/>
+        <f>ROUND(E3+B$17, 0)</f>
         <v>-74</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -782,19 +782,19 @@
         <v>-3.2755491999999999</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(D4-B$17, 0)</f>
         <v>54</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
+        <f>ROUND(E4-$B$17, 0)</f>
         <v>-5</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="2"/>
+        <f>ROUND(D4+B$17, 0)</f>
         <v>58</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="3"/>
+        <f>ROUND(E4+B$17, 0)</f>
         <v>-1</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -803,514 +803,514 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1">
+        <v>24.1198382</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-110.42383890000001</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4">
+        <f>ROUND(D5-B$17, 0)</f>
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10.646162</v>
-      </c>
-      <c r="E5" s="2">
-        <v>61.408810600000002</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>59</v>
+        <f>ROUND(E5-$B$17, 0)</f>
+        <v>-112</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f>ROUND(D5+B$17, 0)</f>
+        <v>26</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="3"/>
-        <v>63</v>
+        <f>ROUND(E5+B$17, 0)</f>
+        <v>-108</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1">
-        <v>24.1198382</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-110.42383890000001</v>
+        <v>39.947862000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>116.29118889999999</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f>ROUND(D6-B$17, 0)</f>
+        <v>38</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>-112</v>
+        <f>ROUND(E6-$B$17, 0)</f>
+        <v>114</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>ROUND(D6+B$17, 0)</f>
+        <v>42</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="3"/>
-        <v>-108</v>
+        <f>ROUND(E6+B$17, 0)</f>
+        <v>118</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1">
-        <v>39.947862000000001</v>
-      </c>
-      <c r="E7" s="2">
-        <v>116.29118889999999</v>
+        <v>45.084285999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-67.079771100000002</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f>ROUND(D7-B$17, 0)</f>
+        <v>43</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>114</v>
+        <f>ROUND(E7-$B$17, 0)</f>
+        <v>-69</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f>ROUND(D7+B$17, 0)</f>
+        <v>47</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
+        <f>ROUND(E7+B$17, 0)</f>
+        <v>-65</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1">
-        <v>45.084285999999999</v>
+        <v>39.747138900000003</v>
       </c>
       <c r="E8" s="1">
-        <v>-67.079771100000002</v>
+        <v>141.12092100000001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <f>ROUND(D8-B$17, 0)</f>
+        <v>38</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="1"/>
-        <v>-69</v>
+        <f>ROUND(E8-$B$17, 0)</f>
+        <v>139</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>47</v>
+        <f>ROUND(D8+B$17, 0)</f>
+        <v>42</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="3"/>
-        <v>-65</v>
+        <f>ROUND(E8+B$17, 0)</f>
+        <v>143</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1">
-        <v>39.747138900000003</v>
+        <v>52.530391600000002</v>
       </c>
       <c r="E9" s="1">
-        <v>141.12092100000001</v>
+        <v>13.409560900000001</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="4">
+        <f>ROUND(D9-B$17, 0)</f>
         <v>51</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
       <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>139</v>
+        <f>ROUND(E9-$B$17, 0)</f>
+        <v>11</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f>ROUND(D9+B$17, 0)</f>
+        <v>55</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="3"/>
-        <v>143</v>
+        <f>ROUND(E9+B$17, 0)</f>
+        <v>15</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1">
-        <v>52.530391600000002</v>
+        <v>14.1547751</v>
       </c>
       <c r="E10" s="1">
-        <v>13.409560900000001</v>
+        <v>121.18415539999999</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <f>ROUND(D10-B$17, 0)</f>
+        <v>12</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f>ROUND(E10-$B$17, 0)</f>
+        <v>119</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f>ROUND(D10+B$17, 0)</f>
+        <v>16</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f>ROUND(E10+B$17, 0)</f>
+        <v>123</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1">
-        <v>14.1547751</v>
+        <v>30.7249938</v>
       </c>
       <c r="E11" s="1">
-        <v>121.18415539999999</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
+        <v>78.411376300000001</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>ROUND(D11-B$17, 0)</f>
+        <v>29</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>119</v>
+        <f>ROUND(E11-$B$17, 0)</f>
+        <v>76</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f>ROUND(D11+B$17, 0)</f>
+        <v>33</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="3"/>
-        <v>123</v>
+        <f>ROUND(E11+B$17, 0)</f>
+        <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1">
+        <v>55.705708399999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.5956285</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="4">
+        <f>ROUND(D12-B$17, 0)</f>
         <v>54</v>
       </c>
-      <c r="D12" s="1">
-        <v>30.7249938</v>
-      </c>
-      <c r="E12" s="1">
-        <v>78.411376300000001</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>76</v>
+        <f>ROUND(E12-$B$17, 0)</f>
+        <v>11</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f>ROUND(D12+B$17, 0)</f>
+        <v>58</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="3"/>
-        <v>80</v>
+        <f>ROUND(E12+B$17, 0)</f>
+        <v>15</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1">
-        <v>55.705708399999999</v>
+        <v>-24.660585399999999</v>
       </c>
       <c r="E13" s="1">
-        <v>12.5956285</v>
+        <v>25.928716099999999</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <f>ROUND(D13-B$17, 0)</f>
+        <v>-27</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f>ROUND(E13-$B$17, 0)</f>
+        <v>24</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f>ROUND(D13+B$17, 0)</f>
+        <v>-23</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f>ROUND(E13+B$17, 0)</f>
+        <v>28</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="D14" s="1">
-        <v>-24.660585399999999</v>
+        <v>51.194041300000002</v>
       </c>
       <c r="E14" s="1">
-        <v>25.928716099999999</v>
+        <v>-0.8247681</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>-27</v>
+        <f>ROUND(D14-B$17, 0)</f>
+        <v>49</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f>ROUND(E14-$B$17, 0)</f>
+        <v>-3</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="2"/>
-        <v>-23</v>
+        <f>ROUND(D14+B$17, 0)</f>
+        <v>53</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="3"/>
-        <v>28</v>
+        <f>ROUND(E14+B$17, 0)</f>
+        <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D15" s="1">
-        <v>51.194041300000002</v>
+        <v>53.533258600000003</v>
       </c>
       <c r="E15" s="1">
-        <v>-0.8247681</v>
+        <v>8.5783214999999995</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G15" s="4">
+        <f t="shared" ref="G15:G16" si="0">ROUND(D15-B$17, 0)</f>
+        <v>52</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" ref="H15:H16" si="1">ROUND(E15-$B$17, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" ref="I15:I16" si="2">ROUND(D15+B$17, 0)</f>
+        <v>56</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" ref="J15:J16" si="3">ROUND(E15+B$17, 0)</f>
+        <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-29.883957200000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>30.591979800000001</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="H15" s="4">
+        <v>-32</v>
+      </c>
+      <c r="H16" s="4">
         <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-      <c r="I15" s="4">
+        <v>29</v>
+      </c>
+      <c r="I16" s="4">
         <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-      <c r="J15" s="4">
+        <v>-28</v>
+      </c>
+      <c r="J16" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="1">
-        <v>53.533258600000003</v>
-      </c>
-      <c r="E16" s="1">
-        <v>8.5783214999999995</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" ref="G16:G17" si="4">ROUND(D16-B$18, 0)</f>
-        <v>52</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" ref="H16:H17" si="5">ROUND(E16-$B$18, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" ref="I16:I17" si="6">ROUND(D16+B$18, 0)</f>
-        <v>56</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" ref="J16:J17" si="7">ROUND(E16+B$18, 0)</f>
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="1">
-        <v>-29.883957200000001</v>
-      </c>
-      <c r="E17" s="1">
-        <v>30.591979800000001</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="4"/>
-        <v>-32</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="6"/>
-        <v>-28</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="7"/>
-        <v>33</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B17" s="7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10.646162</v>
+      </c>
+      <c r="E19" s="2">
+        <v>61.408810600000002</v>
+      </c>
+      <c r="G19" s="4">
+        <f>ROUND(D19-B$17, 0)</f>
+        <v>9</v>
+      </c>
+      <c r="H19" s="4">
+        <f>ROUND(E19-$B$17, 0)</f>
+        <v>59</v>
+      </c>
+      <c r="I19" s="4">
+        <f>ROUND(D19+B$17, 0)</f>
+        <v>13</v>
+      </c>
+      <c r="J19" s="4">
+        <f>ROUND(E19+B$17, 0)</f>
+        <v>63</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>